<commit_message>
new Sinhala words for new timer block
</commit_message>
<xml_diff>
--- a/src/locale/locale.xlsx
+++ b/src/locale/locale.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="242">
   <si>
     <t>Language-Name</t>
   </si>
@@ -529,9 +529,6 @@
     <t>%s වචනයේ දිග</t>
   </si>
   <si>
-    <t>illumination : %s % at %d.sockets socket</t>
-  </si>
-  <si>
     <t>User Logged in Successfully!</t>
   </si>
   <si>
@@ -721,9 +718,6 @@
     <t xml:space="preserve">%d.state කරන්න, %d.sockets හි ස්විචය  </t>
   </si>
   <si>
-    <t xml:space="preserve">දීප්තිය : %s, %d.sockets  හි </t>
-  </si>
-  <si>
     <t>විජට් සකසන්න</t>
   </si>
   <si>
@@ -760,22 +754,34 @@
     <t xml:space="preserve">%d.sockets සොකට්ටුවෙන් Horusහි උෂ්ණත්වය කියවන්න </t>
   </si>
   <si>
-    <t xml:space="preserve">control switch at %d.sockets via timer %d.timers </t>
-  </si>
-  <si>
     <t>read value at %d.yellow from Theia</t>
   </si>
   <si>
     <t>%d.yellow හි ඇති Theia අගය කියවන්න</t>
   </si>
   <si>
-    <t>%d.sockets සොකට්ටුව %d.timers මගින් පාලනය කරන්න</t>
-  </si>
-  <si>
     <t>commiunicate as %m.widgetMqttTopics</t>
   </si>
   <si>
     <t xml:space="preserve">%m.widgetMqttTopics ලෙස සන්නිවේදනය කරන්න </t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off device at %d.sockets via timer %d.timers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on device at %d.sockets via timer %d.timers </t>
+  </si>
+  <si>
+    <t>%d.sockets සොකට්ටුව %d.timers මගින් ඕෆ් කරන්න</t>
+  </si>
+  <si>
+    <t>%d.sockets සොකට්ටුව %d.timers මගින් ඔන් කරන්න</t>
+  </si>
+  <si>
+    <t>set illumination : %s % at %d.sockets socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">දීප්තිය : %s, %d.sockets  හි ලෙස </t>
   </si>
 </sst>
 </file>
@@ -1482,6 +1488,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3314700</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10963275" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3314700</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10963275" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1775,10 +1877,10 @@
   <dimension ref="A1:T235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A124" sqref="A124"/>
+      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="15" customHeight="1"/>
@@ -2060,7 +2162,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
@@ -2196,7 +2298,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C19" s="3"/>
       <c r="M19" s="3"/>
@@ -2569,7 +2671,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
@@ -2913,7 +3015,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
@@ -3033,7 +3135,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
@@ -3181,28 +3283,28 @@
     </row>
     <row r="68" spans="1:17" ht="13.5" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q68" s="6"/>
     </row>
     <row r="69" spans="1:17" ht="13.5" customHeight="1">
       <c r="A69" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="Q69" s="6"/>
     </row>
     <row r="70" spans="1:17" ht="13.5" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q70" s="6"/>
     </row>
@@ -3256,7 +3358,7 @@
         <v>105</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q76" s="6"/>
     </row>
@@ -3346,7 +3448,7 @@
         <v>131</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q86" s="6"/>
     </row>
@@ -3355,133 +3457,133 @@
         <v>132</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q87" s="6"/>
     </row>
     <row r="88" spans="1:17" ht="13.5" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="Q88" s="6"/>
     </row>
     <row r="89" spans="1:17" ht="13.5" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>157</v>
+        <v>240</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="Q89" s="6"/>
     </row>
     <row r="90" spans="1:17" ht="13.5" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q90" s="6"/>
     </row>
     <row r="91" spans="1:17" ht="13.5" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q91" s="6"/>
     </row>
     <row r="92" spans="1:17" ht="13.5" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q92" s="6"/>
     </row>
     <row r="93" spans="1:17" ht="13.5" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q93" s="6"/>
     </row>
     <row r="94" spans="1:17" ht="13.5" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q94" s="6"/>
     </row>
     <row r="95" spans="1:17" ht="13.5" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q95" s="6"/>
     </row>
     <row r="96" spans="1:17" ht="13.5" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q96" s="6"/>
     </row>
     <row r="97" spans="1:17" ht="13.5" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q97" s="6"/>
     </row>
     <row r="98" spans="1:17" ht="13.5" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q98" s="6"/>
     </row>
     <row r="99" spans="1:17" ht="13.5" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q99" s="6"/>
     </row>
     <row r="100" spans="1:17" ht="13.5" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q100" s="6"/>
     </row>
     <row r="101" spans="1:17" ht="13.5" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q101" s="6"/>
     </row>
@@ -3490,103 +3592,103 @@
         <v>22</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q102" s="6"/>
     </row>
     <row r="103" spans="1:17" ht="13.5" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q103" s="6"/>
     </row>
     <row r="104" spans="1:17" ht="13.5" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q104" s="6"/>
     </row>
     <row r="105" spans="1:17" ht="13.5" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q105" s="6"/>
     </row>
     <row r="106" spans="1:17" ht="13.5" customHeight="1">
       <c r="A106" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="Q106" s="6"/>
     </row>
     <row r="107" spans="1:17" ht="13.5" customHeight="1">
       <c r="A107" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="Q107" s="6"/>
     </row>
     <row r="108" spans="1:17" ht="13.5" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q108" s="6"/>
     </row>
     <row r="109" spans="1:17" ht="13.5" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q109" s="6"/>
     </row>
     <row r="110" spans="1:17" ht="13.5" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q110" s="6"/>
     </row>
     <row r="111" spans="1:17" ht="13.5" customHeight="1">
       <c r="A111" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="Q111" s="6"/>
     </row>
     <row r="112" spans="1:17" ht="13.5" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q112" s="6"/>
     </row>
     <row r="113" spans="1:17" ht="13.5" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>63</v>
@@ -3595,16 +3697,16 @@
     </row>
     <row r="114" spans="1:17" ht="13.5" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q114" s="6"/>
     </row>
     <row r="115" spans="1:17" ht="13.5" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>117</v>
@@ -3613,77 +3715,83 @@
     </row>
     <row r="116" spans="1:17" ht="13.5" customHeight="1">
       <c r="A116" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="Q116" s="6"/>
     </row>
     <row r="117" spans="1:17" ht="13.5" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="Q117" s="6"/>
     </row>
     <row r="118" spans="1:17" ht="13.5" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q118" s="6"/>
     </row>
     <row r="119" spans="1:17" ht="13.5" customHeight="1">
       <c r="A119" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="Q119" s="6"/>
     </row>
     <row r="120" spans="1:17" ht="13.5" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="Q120" s="6"/>
     </row>
     <row r="121" spans="1:17" ht="13.5" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q121" s="6"/>
     </row>
     <row r="122" spans="1:17" ht="13.5" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="Q122" s="6"/>
     </row>
     <row r="123" spans="1:17" ht="13.5" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q123" s="6"/>
+    </row>
+    <row r="124" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A124" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="Q123" s="6"/>
-    </row>
-    <row r="124" spans="1:17" ht="13.5" customHeight="1">
+      <c r="B124" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="Q124" s="6"/>
     </row>
     <row r="125" spans="1:17" ht="13.5" customHeight="1">

</xml_diff>